<commit_message>
Update Rizka - Admin Login
</commit_message>
<xml_diff>
--- a/Data Binding_Rizka.xlsx
+++ b/Data Binding_Rizka.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\LearningManagementWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E796D9-1430-437F-97DB-579BDD065A4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2920428D-EB40-4CBB-B552-8BECA43C936A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
   </bookViews>
@@ -425,7 +425,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Rizka - Admin Manage Test Quiz
</commit_message>
<xml_diff>
--- a/Data Binding_Rizka.xlsx
+++ b/Data Binding_Rizka.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\LearningManagementWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2920428D-EB40-4CBB-B552-8BECA43C936A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A787B579-A675-4EE7-B02C-38F78E7EAF4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin - Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Admin - Quiz - Edit" sheetId="2" r:id="rId2"/>
+    <sheet name="Admin - Quiz - Delete" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t>username</t>
   </si>
@@ -63,13 +65,124 @@
   </si>
   <si>
     <t>Pas</t>
+  </si>
+  <si>
+    <t>soalQuestion</t>
+  </si>
+  <si>
+    <t>tipeSoal</t>
+  </si>
+  <si>
+    <t>jobFunction</t>
+  </si>
+  <si>
+    <t>jobPosition</t>
+  </si>
+  <si>
+    <t>module</t>
+  </si>
+  <si>
+    <t>subModule</t>
+  </si>
+  <si>
+    <t>technicalCompetence</t>
+  </si>
+  <si>
+    <t>levelCompetence</t>
+  </si>
+  <si>
+    <t>kunciJawaban</t>
+  </si>
+  <si>
+    <t>jawabanA</t>
+  </si>
+  <si>
+    <t>jawabanB</t>
+  </si>
+  <si>
+    <t>jawabanC</t>
+  </si>
+  <si>
+    <t>jawabanD</t>
+  </si>
+  <si>
+    <t>uraian</t>
+  </si>
+  <si>
+    <t>Pilihan Ganda</t>
+  </si>
+  <si>
+    <t>SALES</t>
+  </si>
+  <si>
+    <t>SALES HEAD</t>
+  </si>
+  <si>
+    <t>NEOP Sales</t>
+  </si>
+  <si>
+    <t>(Asuransi) Apa saja yang dijual?</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Benar</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Mobil</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Truk</t>
+  </si>
+  <si>
+    <t>Kelapa Sawit</t>
+  </si>
+  <si>
+    <t>Apa yang ditawarkan ACC?</t>
+  </si>
+  <si>
+    <t>kunciJawabanPilgan</t>
+  </si>
+  <si>
+    <t>Benar / Salah</t>
+  </si>
+  <si>
+    <t>Uraian</t>
+  </si>
+  <si>
+    <t>Uang kartal adalah ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alat yang sah yang digunakan sebagai pengganti uang karena lebih praktis dan ekonomis. Tetapi tidak berlaku mutlak sebagai alat pengukur karena dapat ditolak  tanpa adanya sanksi hukum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uang kartal adalah alat yang sah yang digunakan sebagai pengganti uang karena lebih praktis dan ekonomis. Tetapi tidak berlaku mutlak sebagai alat pengukur karena dapat ditolak  tanpa adanya sanksi hukum </t>
+  </si>
+  <si>
+    <t>SALES MANAGER</t>
+  </si>
+  <si>
+    <t>BRANCH MANAGER</t>
+  </si>
+  <si>
+    <t>NEOP RCCA</t>
+  </si>
+  <si>
+    <t>NEOP ARHO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,19 +198,71 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -106,8 +271,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530BF696-3D8C-4503-B72B-B5311749EF17}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,72 +615,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>11666</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>11666</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>11688</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>11666</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -509,4 +688,242 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15713736-89B0-4CD9-B732-735568246817}">
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB17C08-6D84-4C26-8E87-CCCE15F7115E}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Rizka - Logout dan Quiz-Edit
</commit_message>
<xml_diff>
--- a/Data Binding_Rizka.xlsx
+++ b/Data Binding_Rizka.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\LearningManagementWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A787B579-A675-4EE7-B02C-38F78E7EAF4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116B8C66-EA86-4789-A41C-E1B80743BB93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13410" windowHeight="11070" firstSheet="1" activeTab="1" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin - Login" sheetId="1" r:id="rId1"/>
     <sheet name="Admin - Quiz - Edit" sheetId="2" r:id="rId2"/>
     <sheet name="Admin - Quiz - Delete" sheetId="3" r:id="rId3"/>
+    <sheet name="Admin - Logout" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>username</t>
   </si>
@@ -124,9 +125,6 @@
     <t>(Asuransi) Apa saja yang dijual?</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Benar</t>
   </si>
   <si>
@@ -176,6 +174,21 @@
   </si>
   <si>
     <t>NEOP ARHO</t>
+  </si>
+  <si>
+    <t>Post-Test</t>
+  </si>
+  <si>
+    <t>Belajar apa aja kita?</t>
+  </si>
+  <si>
+    <t>Lalala</t>
+  </si>
+  <si>
+    <t>Nanana</t>
+  </si>
+  <si>
+    <t>Kakaka</t>
   </si>
 </sst>
 </file>
@@ -207,7 +220,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,6 +242,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -286,6 +305,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15713736-89B0-4CD9-B732-735568246817}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,7 +783,7 @@
         <v>22</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>23</v>
@@ -784,29 +809,29 @@
         <v>28</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="N2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3" t="s">
@@ -815,31 +840,31 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -853,28 +878,28 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -883,7 +908,7 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>4</v>
@@ -898,7 +923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB17C08-6D84-4C26-8E87-CCCE15F7115E}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -926,4 +951,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A072F818-9552-4EDA-9FA3-7B54FF4CDAE5}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Rizka - Admin Quiz Delete
</commit_message>
<xml_diff>
--- a/Data Binding_Rizka.xlsx
+++ b/Data Binding_Rizka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\LearningManagementWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116B8C66-EA86-4789-A41C-E1B80743BB93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBDA6EB-FE4B-478B-A1D7-222F182D48A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13410" windowHeight="11070" firstSheet="1" activeTab="1" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13410" windowHeight="11070" firstSheet="1" activeTab="2" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin - Login" sheetId="1" r:id="rId1"/>
@@ -719,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15713736-89B0-4CD9-B732-735568246817}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -923,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB17C08-6D84-4C26-8E87-CCCE15F7115E}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,13 +938,13 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Rizka - Manage Modules - Search
</commit_message>
<xml_diff>
--- a/Data Binding_Rizka.xlsx
+++ b/Data Binding_Rizka.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\LearningManagementWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBDA6EB-FE4B-478B-A1D7-222F182D48A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D56CD7D-B430-4A4F-80A5-5DE34CD2531D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13410" windowHeight="11070" firstSheet="1" activeTab="2" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13410" windowHeight="11070" firstSheet="2" activeTab="3" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin - Login" sheetId="1" r:id="rId1"/>
     <sheet name="Admin - Quiz - Edit" sheetId="2" r:id="rId2"/>
     <sheet name="Admin - Quiz - Delete" sheetId="3" r:id="rId3"/>
-    <sheet name="Admin - Logout" sheetId="4" r:id="rId4"/>
+    <sheet name="Admin - Manage Modules" sheetId="5" r:id="rId4"/>
+    <sheet name="Admin - Logout" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>username</t>
   </si>
@@ -189,6 +190,18 @@
   </si>
   <si>
     <t>Kakaka</t>
+  </si>
+  <si>
+    <t>namaModul</t>
+  </si>
+  <si>
+    <t>security testing !@#$%^&amp;*()__+_)</t>
+  </si>
+  <si>
+    <t>NEOP Teller Cash &amp; PDC, dan FAB</t>
+  </si>
+  <si>
+    <t>Karyawan baru pada fungsi AR</t>
   </si>
 </sst>
 </file>
@@ -290,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -311,6 +324,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -923,7 +940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB17C08-6D84-4C26-8E87-CCCE15F7115E}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -954,6 +971,60 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{720D1816-83D2-4B85-85C4-B677AD756BBD}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A072F818-9552-4EDA-9FA3-7B54FF4CDAE5}">
   <dimension ref="A1:A2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update Rizka - Admin - Change Password & Next Page
</commit_message>
<xml_diff>
--- a/Data Binding_Rizka.xlsx
+++ b/Data Binding_Rizka.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\LearningManagementWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D56CD7D-B430-4A4F-80A5-5DE34CD2531D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C16202A-B6DC-447A-9634-7C5CE2ADDFBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13410" windowHeight="11070" firstSheet="2" activeTab="3" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
+    <workbookView xWindow="6180" yWindow="15" windowWidth="13410" windowHeight="11055" firstSheet="2" activeTab="4" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin - Login" sheetId="1" r:id="rId1"/>
     <sheet name="Admin - Quiz - Edit" sheetId="2" r:id="rId2"/>
     <sheet name="Admin - Quiz - Delete" sheetId="3" r:id="rId3"/>
     <sheet name="Admin - Manage Modules" sheetId="5" r:id="rId4"/>
-    <sheet name="Admin - Logout" sheetId="4" r:id="rId5"/>
+    <sheet name="Admin - Change Password" sheetId="6" r:id="rId5"/>
+    <sheet name="Admin - Logout" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
   <si>
     <t>username</t>
   </si>
@@ -202,6 +203,27 @@
   </si>
   <si>
     <t>Karyawan baru pada fungsi AR</t>
+  </si>
+  <si>
+    <t>currentPassword</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
+    <t>confirmPassword</t>
+  </si>
+  <si>
+    <t>lalalala</t>
+  </si>
+  <si>
+    <t>cancelSave</t>
+  </si>
+  <si>
+    <t>A123456</t>
+  </si>
+  <si>
+    <t>Aa123456</t>
   </si>
 </sst>
 </file>
@@ -233,7 +255,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,6 +283,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -328,6 +356,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -974,7 +1005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{720D1816-83D2-4B85-85C4-B677AD756BBD}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -1025,6 +1056,94 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C76323-15BF-4A39-98D1-F5CE8C19E7AE}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A072F818-9552-4EDA-9FA3-7B54FF4CDAE5}">
   <dimension ref="A1:A2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update Rizka - 26 Mei 2020
</commit_message>
<xml_diff>
--- a/Data Binding_Rizka.xlsx
+++ b/Data Binding_Rizka.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\LearningManagementWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C16202A-B6DC-447A-9634-7C5CE2ADDFBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BCDEC8-A50A-4C42-8E77-C0E2CCFE72C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="15" windowWidth="13410" windowHeight="11055" firstSheet="2" activeTab="4" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
+    <workbookView xWindow="1350" yWindow="105" windowWidth="13410" windowHeight="11055" firstSheet="5" activeTab="6" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin - Login" sheetId="1" r:id="rId1"/>
     <sheet name="Admin - Quiz - Edit" sheetId="2" r:id="rId2"/>
     <sheet name="Admin - Quiz - Delete" sheetId="3" r:id="rId3"/>
-    <sheet name="Admin - Manage Modules" sheetId="5" r:id="rId4"/>
+    <sheet name="Admin - Manage Modules - Search" sheetId="5" r:id="rId4"/>
     <sheet name="Admin - Change Password" sheetId="6" r:id="rId5"/>
     <sheet name="Admin - Logout" sheetId="4" r:id="rId6"/>
+    <sheet name="Admin - Quiz - Search" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
   <si>
     <t>username</t>
   </si>
@@ -224,6 +225,15 @@
   </si>
   <si>
     <t>Aa123456</t>
+  </si>
+  <si>
+    <t>judulQuiz</t>
+  </si>
+  <si>
+    <t>ABC lima dasar</t>
+  </si>
+  <si>
+    <t>Salah satu lini Bisnis Astra adalah ...</t>
   </si>
 </sst>
 </file>
@@ -255,7 +265,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,6 +299,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -358,6 +374,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1006,7 +1037,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C76323-15BF-4A39-98D1-F5CE8C19E7AE}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,4 +1198,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30DABA46-5CDF-46BA-8077-2E98F39AA10E}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Rizka - 27 Mei 2020
</commit_message>
<xml_diff>
--- a/Data Binding_Rizka.xlsx
+++ b/Data Binding_Rizka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\LearningManagementWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CD2B21-EEC4-4CE7-BD5A-3DA32A18C2F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF86CE1A-DD5C-4B0C-ACE1-9DE959DADD59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="315" windowWidth="13410" windowHeight="11055" activeTab="2" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin - Login" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="71">
   <si>
     <t>username</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Coba ya</t>
+  </si>
+  <si>
+    <t>isEmpty</t>
   </si>
 </sst>
 </file>
@@ -369,16 +372,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -413,8 +414,23 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530BF696-3D8C-4503-B72B-B5311749EF17}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,16 +760,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -811,6 +827,30 @@
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>11666</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -823,198 +863,198 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15713736-89B0-4CD9-B732-735568246817}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.85546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="44.7109375" style="4" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="17" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3" t="s">
+      <c r="O2" s="18"/>
+      <c r="P2" s="18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3" t="s">
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3" t="s">
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="18" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1027,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4068243B-B4DE-45C8-9E55-386E38B1F7C1}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,168 +1090,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="17" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="14" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14" t="s">
+      <c r="I2" s="21"/>
+      <c r="J2" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14" t="s">
+      <c r="O2" s="21"/>
+      <c r="P2" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="14" t="s">
+      <c r="G3" s="22"/>
+      <c r="H3" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14" t="s">
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="21">
         <v>12</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14" t="s">
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1234,17 +1274,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1259,7 +1299,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,10 +1308,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1300,8 +1340,8 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1325,16 +1365,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1407,12 +1447,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1436,26 +1476,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Rizka - 28 Mei 2020
</commit_message>
<xml_diff>
--- a/Data Binding_Rizka.xlsx
+++ b/Data Binding_Rizka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\LearningManagementWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF86CE1A-DD5C-4B0C-ACE1-9DE959DADD59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC57D54E-A065-48FA-AD89-1B547D2CE72B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin - Login" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="79">
   <si>
     <t>username</t>
   </si>
@@ -186,9 +186,6 @@
     <t>Belajar apa aja kita?</t>
   </si>
   <si>
-    <t>Lalala</t>
-  </si>
-  <si>
     <t>Nanana</t>
   </si>
   <si>
@@ -253,6 +250,33 @@
   </si>
   <si>
     <t>isEmpty</t>
+  </si>
+  <si>
+    <t>LALALALA</t>
+  </si>
+  <si>
+    <t>New Question (4)</t>
+  </si>
+  <si>
+    <t>New Question (5)</t>
+  </si>
+  <si>
+    <t>New Question (6)</t>
+  </si>
+  <si>
+    <t>New Question (7)</t>
+  </si>
+  <si>
+    <t>New Question (8)</t>
+  </si>
+  <si>
+    <t>New Question (9)</t>
+  </si>
+  <si>
+    <t>New Question (10)</t>
+  </si>
+  <si>
+    <t>Alfabet</t>
   </si>
 </sst>
 </file>
@@ -372,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -432,6 +456,16 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530BF696-3D8C-4503-B72B-B5311749EF17}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,7 +872,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -850,7 +884,17 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -861,10 +905,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15713736-89B0-4CD9-B732-735568246817}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,7 +927,8 @@
     <col min="13" max="13" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="44.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="4"/>
+    <col min="16" max="16" width="9.140625" style="4" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -952,12 +997,8 @@
       <c r="E2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>48</v>
-      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
       <c r="H2" s="20" t="s">
         <v>35</v>
       </c>
@@ -999,11 +1040,9 @@
         <v>46</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>49</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="G3" s="24"/>
       <c r="H3" s="19" t="s">
         <v>41</v>
       </c>
@@ -1037,10 +1076,10 @@
         <v>47</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="G4" s="18">
+        <v>12</v>
       </c>
       <c r="H4" s="19" t="s">
         <v>39</v>
@@ -1058,6 +1097,44 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1065,10 +1142,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4068243B-B4DE-45C8-9E55-386E38B1F7C1}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1157,7 @@
     <col min="5" max="5" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -1158,7 +1235,7 @@
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
       <c r="H2" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I2" s="21"/>
       <c r="J2" s="21" t="s">
@@ -1181,7 +1258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>37</v>
       </c>
@@ -1197,15 +1274,15 @@
       <c r="E3" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="21">
+        <v>12</v>
+      </c>
       <c r="H3" s="21" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
@@ -1234,16 +1311,14 @@
         <v>46</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="21">
-        <v>12</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="G4" s="22"/>
       <c r="H4" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="J4" s="21"/>
       <c r="K4" s="21"/>
@@ -1255,7 +1330,388 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="21">
+        <v>12</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="21">
+        <v>12</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="23">
+        <v>12</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="22"/>
+      <c r="F8" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="23">
+        <v>12</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="23">
+        <v>12</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="23">
+        <v>12</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="23">
+        <v>12</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="22"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23">
+        <v>12</v>
+      </c>
+      <c r="H12" s="22"/>
+      <c r="I12" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1299,7 +1755,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,7 +1765,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>2</v>
@@ -1317,7 +1773,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -1325,7 +1781,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -1333,7 +1789,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
@@ -1366,13 +1822,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>56</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>57</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>2</v>
@@ -1397,13 +1853,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1411,10 +1867,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -1477,7 +1933,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>2</v>
@@ -1485,7 +1941,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>4</v>
@@ -1493,7 +1949,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Update Rizka - 17 Juni 2020
</commit_message>
<xml_diff>
--- a/Data Binding_Rizka.xlsx
+++ b/Data Binding_Rizka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\LearningManagementWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB10CD94-4A66-4652-9252-EE7281E25FB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C550C6C9-0545-4EA4-ADBC-2BE2CB000B64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="2" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="3" activeTab="5" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin - Login" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="94">
   <si>
     <t>username</t>
   </si>
@@ -207,9 +207,6 @@
     <t>cancelSave</t>
   </si>
   <si>
-    <t>A123456</t>
-  </si>
-  <si>
     <t>Aa123456</t>
   </si>
   <si>
@@ -298,6 +295,33 @@
   </si>
   <si>
     <t>Edit (11)</t>
+  </si>
+  <si>
+    <t>Password4</t>
+  </si>
+  <si>
+    <t>ket</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>#AAAAAAA</t>
+  </si>
+  <si>
+    <t>OTPSalah</t>
+  </si>
+  <si>
+    <t>notMatch</t>
+  </si>
+  <si>
+    <t>currentPassWrong</t>
+  </si>
+  <si>
+    <t>#.1234567</t>
+  </si>
+  <si>
+    <t>#,1234567A</t>
   </si>
 </sst>
 </file>
@@ -391,7 +415,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -414,11 +438,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -498,6 +533,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,7 +853,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +942,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -916,7 +954,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -926,7 +964,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1032,7 +1070,7 @@
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
       <c r="H2" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I2" s="26"/>
       <c r="J2" s="26" t="s">
@@ -1074,7 +1112,7 @@
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="H3" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I3" s="26"/>
       <c r="J3" s="26" t="s">
@@ -1112,7 +1150,7 @@
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I4" s="18" t="s">
         <v>29</v>
@@ -1150,7 +1188,7 @@
         <v>12</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I5" s="28"/>
       <c r="J5" s="28"/>
@@ -1159,7 +1197,7 @@
       <c r="M5" s="28"/>
       <c r="N5" s="28"/>
       <c r="O5" s="29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P5" s="28" t="s">
         <v>4</v>
@@ -1188,7 +1226,7 @@
         <v>12</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
@@ -1224,7 +1262,7 @@
         <v>12</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I7" s="18" t="s">
         <v>29</v>
@@ -1254,16 +1292,16 @@
         <v>42</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G8" s="18">
         <v>12</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J8" s="18"/>
       <c r="K8" s="18"/>
@@ -1288,13 +1326,13 @@
         <v>42</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G9" s="18">
         <v>12</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I9" s="18" t="s">
         <v>29</v>
@@ -1324,16 +1362,16 @@
         <v>42</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G10" s="18">
         <v>12</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
@@ -1360,13 +1398,13 @@
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G11" s="18">
         <v>12</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I11" s="18" t="s">
         <v>29</v>
@@ -1394,16 +1432,16 @@
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
       <c r="F12" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G12" s="18">
         <v>12</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
@@ -1424,13 +1462,13 @@
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G13" s="18">
         <v>12</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" s="18" t="s">
         <v>29</v>
@@ -1467,7 +1505,7 @@
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J14" s="18"/>
       <c r="K14" s="18"/>
@@ -1496,7 +1534,7 @@
         <v>42</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
@@ -1533,7 +1571,7 @@
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
       <c r="I16" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
@@ -1562,13 +1600,13 @@
         <v>42</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I17" s="18" t="s">
         <v>29</v>
@@ -1592,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4068243B-B4DE-45C8-9E55-386E38B1F7C1}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1683,7 +1721,7 @@
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
       <c r="H2" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I2" s="18"/>
       <c r="J2" s="18" t="s">
@@ -1727,10 +1765,10 @@
         <v>12</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
@@ -1759,11 +1797,11 @@
         <v>42</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I4" s="18" t="s">
         <v>29</v>
@@ -1793,16 +1831,16 @@
         <v>42</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G5" s="18">
         <v>12</v>
       </c>
       <c r="H5" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" s="18" t="s">
         <v>62</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>63</v>
       </c>
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
@@ -1827,16 +1865,16 @@
         <v>42</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6" s="18">
         <v>12</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
@@ -1863,13 +1901,13 @@
         <v>42</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G7" s="20">
         <v>12</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I7" s="20" t="s">
         <v>29</v>
@@ -1899,13 +1937,13 @@
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G8" s="20">
         <v>12</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8" s="20" t="s">
         <v>29</v>
@@ -1933,13 +1971,13 @@
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
       <c r="F9" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G9" s="20">
         <v>12</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I9" s="20" t="s">
         <v>29</v>
@@ -1963,16 +2001,16 @@
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
       <c r="F10" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G10" s="20">
         <v>12</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
@@ -2001,13 +2039,13 @@
         <v>42</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G11" s="20">
         <v>12</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I11" s="19"/>
       <c r="J11" s="20"/>
@@ -2071,7 +2109,7 @@
         <v>42</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
@@ -2108,7 +2146,7 @@
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
       <c r="I14" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
@@ -2137,16 +2175,16 @@
         <v>42</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J15" s="20"/>
       <c r="K15" s="20"/>
@@ -2274,10 +2312,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C76323-15BF-4A39-98D1-F5CE8C19E7AE}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2286,9 +2324,10 @@
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>50</v>
       </c>
@@ -2301,58 +2340,244 @@
       <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="E1" s="31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="14">
+        <v>123456</v>
+      </c>
+      <c r="C7" s="14">
+        <v>123456</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2401,7 +2626,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>2</v>
@@ -2409,7 +2634,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>4</v>
@@ -2417,7 +2642,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Update Rizka - 22 Juni 2020
</commit_message>
<xml_diff>
--- a/Data Binding_Rizka.xlsx
+++ b/Data Binding_Rizka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\LearningManagementWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E64E284-36D3-4A33-AC87-B0C492DCD70A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A27BCFC-AE6F-425E-B1DF-DBFFA28516BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="15" windowWidth="13410" windowHeight="11055" firstSheet="4" activeTab="4" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
+    <workbookView xWindow="975" yWindow="15" windowWidth="13410" windowHeight="11055" firstSheet="3" activeTab="3" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin - Login" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="109">
   <si>
     <t>username</t>
   </si>
@@ -361,6 +361,12 @@
   </si>
   <si>
     <t>AsalAjaYa...</t>
+  </si>
+  <si>
+    <t>namaSoal</t>
+  </si>
+  <si>
+    <t>COBA 1</t>
   </si>
 </sst>
 </file>
@@ -2265,29 +2271,38 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB17C08-6D84-4C26-8E87-CCCE15F7115E}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>160708926</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2301,7 +2316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{720D1816-83D2-4B85-85C4-B677AD756BBD}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update Rizka - 25 Juni 2020
</commit_message>
<xml_diff>
--- a/Data Binding_Rizka.xlsx
+++ b/Data Binding_Rizka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\LearningManagementWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A27BCFC-AE6F-425E-B1DF-DBFFA28516BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126F8856-CEE8-4EB6-A2FD-AF27818FC5B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="15" windowWidth="13410" windowHeight="11055" firstSheet="3" activeTab="3" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
+    <workbookView xWindow="975" yWindow="15" windowWidth="13410" windowHeight="11055" firstSheet="6" activeTab="7" xr2:uid="{F9A2B98F-EEE1-4ED4-BB4F-7578AA456839}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin - Login" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="117">
   <si>
     <t>username</t>
   </si>
@@ -201,12 +201,6 @@
     <t>judulQuiz</t>
   </si>
   <si>
-    <t>ABC lima dasar</t>
-  </si>
-  <si>
-    <t>Salah satu lini Bisnis Astra adalah ...</t>
-  </si>
-  <si>
     <t>New Question (1)</t>
   </si>
   <si>
@@ -367,6 +361,36 @@
   </si>
   <si>
     <t>COBA 1</t>
+  </si>
+  <si>
+    <t>benarsalah</t>
+  </si>
+  <si>
+    <t>Giro boleh dikirimkan customer melalui pos atau paket</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Teller</t>
+  </si>
+  <si>
+    <t>NEOP CSO</t>
+  </si>
+  <si>
+    <t>Quiz</t>
+  </si>
+  <si>
+    <t>IT Trainee ACC</t>
+  </si>
+  <si>
+    <t>modul</t>
+  </si>
+  <si>
+    <t>soal</t>
+  </si>
+  <si>
+    <t>tipeTest</t>
   </si>
 </sst>
 </file>
@@ -437,12 +461,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -459,8 +477,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -494,11 +518,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -536,30 +573,33 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -570,18 +610,18 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -989,7 +1029,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1001,7 +1041,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1011,7 +1051,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1049,278 +1089,278 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="O1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" s="15" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="26" t="s">
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="17"/>
+      <c r="L3" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="26">
+        <v>12</v>
+      </c>
+      <c r="H5" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="25" t="s">
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="P5" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="26" t="s">
+      <c r="C6" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="26">
+        <v>12</v>
+      </c>
+      <c r="H6" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="18"/>
-      <c r="L3" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="22" t="s">
+      <c r="G7" s="16">
+        <v>12</v>
+      </c>
+      <c r="H7" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I7" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="27">
-        <v>12</v>
-      </c>
-      <c r="H5" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="P5" s="27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="27">
-        <v>12</v>
-      </c>
-      <c r="H6" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="17">
-        <v>12</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17" t="s">
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1328,35 +1368,35 @@
       <c r="A8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="17" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="17">
+      <c r="F8" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="16">
         <v>12</v>
       </c>
-      <c r="H8" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17" t="s">
+      <c r="H8" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1364,69 +1404,69 @@
       <c r="A9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="17" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="17">
+      <c r="F9" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="16">
         <v>12</v>
       </c>
-      <c r="H9" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I9" s="17" t="s">
+      <c r="H9" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17" t="s">
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="17" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="17">
+      <c r="F10" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="16">
         <v>12</v>
       </c>
-      <c r="H10" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17" t="s">
+      <c r="H10" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1434,35 +1474,35 @@
       <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="17">
+      <c r="E11" s="17"/>
+      <c r="F11" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="16">
         <v>12</v>
       </c>
-      <c r="H11" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="I11" s="17" t="s">
+      <c r="H11" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17" t="s">
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1470,33 +1510,33 @@
       <c r="A12" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="17">
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="16">
         <v>12</v>
       </c>
-      <c r="H12" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17" t="s">
+      <c r="H12" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1504,29 +1544,29 @@
       <c r="A13" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="17">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="16">
         <v>12</v>
       </c>
-      <c r="H13" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="I13" s="17" t="s">
+      <c r="H13" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17" t="s">
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1534,33 +1574,33 @@
       <c r="A14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="17">
+      <c r="F14" s="17"/>
+      <c r="G14" s="16">
         <v>12</v>
       </c>
-      <c r="H14" s="18"/>
-      <c r="I14" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17" t="s">
+      <c r="H14" s="17"/>
+      <c r="I14" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1568,33 +1608,33 @@
       <c r="A15" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="17" t="s">
+      <c r="F15" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17" t="s">
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1602,31 +1642,31 @@
       <c r="A16" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17" t="s">
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1634,37 +1674,37 @@
       <c r="A17" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="I17" s="17" t="s">
+      <c r="F17" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17" t="s">
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1703,49 +1743,49 @@
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="O1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1753,77 +1793,77 @@
       <c r="A2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17" t="s">
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="16"/>
+      <c r="P2" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="17">
+      <c r="F3" s="17"/>
+      <c r="G3" s="16">
         <v>12</v>
       </c>
-      <c r="H3" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17" t="s">
+      <c r="H3" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1831,35 +1871,35 @@
       <c r="A4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="I4" s="17" t="s">
+      <c r="F4" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17" t="s">
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1867,35 +1907,35 @@
       <c r="A5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="17" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" s="17">
+      <c r="F5" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="16">
         <v>12</v>
       </c>
-      <c r="H5" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17" t="s">
+      <c r="H5" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1903,69 +1943,69 @@
       <c r="A6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="17" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="16">
+        <v>12</v>
+      </c>
+      <c r="H6" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="17">
+      <c r="I6" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="18">
         <v>12</v>
       </c>
-      <c r="H6" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" s="19">
-        <v>12</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="I7" s="19" t="s">
+      <c r="H7" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19" t="s">
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1973,35 +2013,35 @@
       <c r="A8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="19">
+      <c r="E8" s="17"/>
+      <c r="F8" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="18">
         <v>12</v>
       </c>
-      <c r="H8" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="19" t="s">
+      <c r="H8" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19" t="s">
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2009,33 +2049,33 @@
       <c r="A9" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="19">
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="18">
         <v>12</v>
       </c>
-      <c r="H9" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="I9" s="19" t="s">
+      <c r="H9" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19" t="s">
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2043,29 +2083,29 @@
       <c r="A10" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="19">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="18">
         <v>12</v>
       </c>
-      <c r="H10" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19" t="s">
+      <c r="H10" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2073,35 +2113,35 @@
       <c r="A11" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="19">
+      <c r="F11" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="18">
         <v>12</v>
       </c>
-      <c r="H11" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19" t="s">
+      <c r="H11" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="17"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2109,33 +2149,33 @@
       <c r="A12" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="19">
+      <c r="F12" s="17"/>
+      <c r="G12" s="18">
         <v>12</v>
       </c>
-      <c r="H12" s="18"/>
-      <c r="I12" s="19" t="s">
+      <c r="H12" s="17"/>
+      <c r="I12" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19" t="s">
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2143,33 +2183,33 @@
       <c r="A13" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="19" t="s">
+      <c r="F13" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19" t="s">
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2177,31 +2217,31 @@
       <c r="A14" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="19" t="s">
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2209,57 +2249,57 @@
       <c r="A15" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19" t="s">
+      <c r="F15" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="29"/>
-      <c r="P16" s="19" t="s">
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2273,7 +2313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB17C08-6D84-4C26-8E87-CCCE15F7115E}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -2284,7 +2324,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
@@ -2292,7 +2332,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -2317,7 +2357,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G12" sqref="G11:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2329,13 +2369,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>90</v>
+        <v>102</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>88</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>2</v>
@@ -2343,13 +2383,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -2357,13 +2397,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
@@ -2371,13 +2411,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
@@ -2385,13 +2425,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
@@ -2399,13 +2439,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>4</v>
@@ -2413,13 +2453,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>4</v>
@@ -2427,13 +2467,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>4</v>
@@ -2441,13 +2481,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
@@ -2464,7 +2504,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2489,8 +2529,8 @@
       <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="30" t="s">
-        <v>82</v>
+      <c r="E1" s="29" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2522,7 +2562,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2537,7 +2577,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2552,7 +2592,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2569,7 +2609,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2586,7 +2626,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2594,16 +2634,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2611,16 +2651,16 @@
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2628,16 +2668,16 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2665,7 +2705,7 @@
         <v>6</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2676,12 +2716,12 @@
         <v>6</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>3</v>
@@ -2693,7 +2733,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2710,7 +2750,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2762,40 +2802,103 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30DABA46-5CDF-46BA-8077-2E98F39AA10E}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="32" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>6</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>